<commit_message>
Filechooser for excel export implemented
</commit_message>
<xml_diff>
--- a/URegister/firstfile.xlsx
+++ b/URegister/firstfile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Datum</t>
   </si>
@@ -41,7 +41,7 @@
     <t>00:00:11</t>
   </si>
   <si>
-    <t>sdfd</t>
+    <t>sdfdtyt</t>
   </si>
   <si>
     <t>18:18:26</t>
@@ -155,6 +155,23 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>